<commit_message>
Updating slides session 5 parts I and I and data
</commit_message>
<xml_diff>
--- a/000_data/005_1_1_1_bp_resumen_iqy.xlsx
+++ b/000_data/005_1_1_1_bp_resumen_iqy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Balanza de pagos de Colombia ¹</t>
   </si>
@@ -46,7 +46,7 @@
         <color theme="1"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>Banco de la República - Gerencia Técnica - información extraída de la bodega de datos -Serankua- el 28/01/2024 13:44:42</t>
+      <t>Banco de la República - Gerencia Técnica - información extraída de la bodega de datos -Serankua- el 16/07/2024 08:40:43</t>
     </r>
   </si>
   <si>
@@ -119,13 +119,16 @@
     <t>2020 (r)</t>
   </si>
   <si>
-    <t>2021 (p)</t>
+    <t>2021 (r)</t>
   </si>
   <si>
     <t>2022 (p)</t>
   </si>
   <si>
-    <t>2023 (pr) (Ene - Sep) *</t>
+    <t>2023 (p)</t>
+  </si>
+  <si>
+    <t>2024 (pr) (Ene - Mar) *</t>
   </si>
   <si>
     <t>1 Cuenta corriente</t>
@@ -556,7 +559,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> * Los datos del año actual corresponden a información de enero a septiembre (año corrido). </t>
+    <t xml:space="preserve"> * Los datos del año actual corresponden a información de enero a marzo (año corrido). </t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1086,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y73"/>
+  <dimension ref="A1:Z73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1092,17 +1095,17 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="95.2381" customWidth="1"/>
-    <col min="2" max="2" width="14.273298" customWidth="1"/>
-    <col min="3" max="3" width="14.273298" customWidth="1"/>
-    <col min="4" max="4" width="13.384405" customWidth="1"/>
-    <col min="5" max="5" width="13.384405" customWidth="1"/>
-    <col min="6" max="6" width="13.384405" customWidth="1"/>
-    <col min="7" max="7" width="13.384405" customWidth="1"/>
-    <col min="8" max="8" width="13.384405" customWidth="1"/>
-    <col min="9" max="9" width="13.384405" customWidth="1"/>
-    <col min="10" max="10" width="13.384394" customWidth="1"/>
-    <col min="11" max="11" width="13.384394" customWidth="1"/>
-    <col min="12" max="12" width="13.384394" customWidth="1"/>
+    <col min="2" max="2" width="14.221667" customWidth="1"/>
+    <col min="3" max="3" width="14.221667" customWidth="1"/>
+    <col min="4" max="4" width="13.332776" customWidth="1"/>
+    <col min="5" max="5" width="13.332776" customWidth="1"/>
+    <col min="6" max="6" width="13.332776" customWidth="1"/>
+    <col min="7" max="7" width="13.332776" customWidth="1"/>
+    <col min="8" max="8" width="13.332776" customWidth="1"/>
+    <col min="9" max="9" width="13.332776" customWidth="1"/>
+    <col min="10" max="10" width="13.332776" customWidth="1"/>
+    <col min="11" max="11" width="13.332776" customWidth="1"/>
+    <col min="12" max="12" width="13.332776" customWidth="1"/>
     <col min="13" max="13" width="12.95238" customWidth="1"/>
     <col min="14" max="14" width="12.95238" customWidth="1"/>
     <col min="15" max="15" width="12.95238" customWidth="1"/>
@@ -1116,7 +1119,8 @@
     <col min="23" max="23" width="12.95238" customWidth="1"/>
     <col min="24" max="24" width="12.952405" customWidth="1"/>
     <col min="25" max="25" width="12.95238" customWidth="1"/>
-    <col min="26" max="26" width="0.7619048" customWidth="1"/>
+    <col min="26" max="26" width="12.95238" customWidth="1"/>
+    <col min="27" max="27" width="0.7619048" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1163,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="16.216" customHeight="1">
+    <row r="10" spans="1:26" ht="16.216" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="19" t="s">
         <v>6</v>
@@ -1190,9 +1194,10 @@
       <c r="V10" s="20"/>
       <c r="W10" s="20"/>
       <c r="X10" s="20"/>
-      <c r="Y10" s="21"/>
-    </row>
-    <row r="11" spans="1:25" ht="56.5" customHeight="1">
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="21"/>
+    </row>
+    <row r="11" spans="1:26" ht="56.5" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -1265,167 +1270,176 @@
       <c r="X11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Y11" s="7" t="s">
+      <c r="Y11" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Z11" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.06" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="11">
         <v>845.40408305</v>
       </c>
       <c r="C12" s="11">
-        <v>-1040.31475186</v>
+        <v>-1040.32792061</v>
       </c>
       <c r="D12" s="11">
-        <v>-1289.1937764</v>
+        <v>-1289.2026699</v>
       </c>
       <c r="E12" s="11">
-        <v>-911.997622326</v>
+        <v>-912.004384376</v>
       </c>
       <c r="F12" s="11">
-        <v>-774.54654289</v>
+        <v>-774.55595089</v>
       </c>
       <c r="G12" s="11">
-        <v>-1947.7435234</v>
+        <v>-1947.7627682</v>
       </c>
       <c r="H12" s="11">
-        <v>-2991.0118031</v>
+        <v>-2991.0365236</v>
       </c>
       <c r="I12" s="11">
-        <v>-6149.613557</v>
+        <v>-6149.638988</v>
       </c>
       <c r="J12" s="11">
-        <v>-6497.270736</v>
+        <v>-6497.285742</v>
       </c>
       <c r="K12" s="11">
-        <v>-4433.0054196</v>
+        <v>-4433.0109261</v>
       </c>
       <c r="L12" s="11">
-        <v>-8583.011648</v>
+        <v>-8583.014198</v>
       </c>
       <c r="M12" s="11">
-        <v>-9734.499319</v>
+        <v>-9734.501794</v>
       </c>
       <c r="N12" s="11">
-        <v>-11639.995687</v>
+        <v>-11639.999051</v>
       </c>
       <c r="O12" s="11">
-        <v>-12365.127742</v>
+        <v>-12365.129749</v>
       </c>
       <c r="P12" s="11">
-        <v>-19818.544018</v>
+        <v>-19818.545633</v>
       </c>
       <c r="Q12" s="11">
-        <v>-18702.227285</v>
+        <v>-18702.229659</v>
       </c>
       <c r="R12" s="11">
-        <v>-12586.55642</v>
+        <v>-12586.561575</v>
       </c>
       <c r="S12" s="11">
-        <v>-9924.358408</v>
+        <v>-9924.365517</v>
       </c>
       <c r="T12" s="11">
-        <v>-14040.948616</v>
+        <v>-14040.960762</v>
       </c>
       <c r="U12" s="11">
-        <v>-14809.636828</v>
+        <v>-14808.667964</v>
       </c>
       <c r="V12" s="11">
-        <v>-9266.80978</v>
+        <v>-9266.813487</v>
       </c>
       <c r="W12" s="11">
-        <v>-17951.185669</v>
+        <v>-17949.402965</v>
       </c>
       <c r="X12" s="11">
-        <v>-21333.262936</v>
-      </c>
-      <c r="Y12" s="12">
-        <v>-7091.927053</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="15.06" customHeight="1">
+        <v>-21204.986317</v>
+      </c>
+      <c r="Y12" s="11">
+        <v>-9153.774491</v>
+      </c>
+      <c r="Z12" s="12">
+        <v>-1924.034491</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.06" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="14">
         <v>18747.7513599</v>
       </c>
       <c r="C13" s="14">
-        <v>18618.5726145</v>
+        <v>18618.5594458</v>
       </c>
       <c r="D13" s="14">
-        <v>17920.3482085</v>
+        <v>17920.339315</v>
       </c>
       <c r="E13" s="14">
-        <v>19854.4202747</v>
+        <v>19854.4135128</v>
       </c>
       <c r="F13" s="14">
-        <v>24335.5447128</v>
+        <v>24335.5353048</v>
       </c>
       <c r="G13" s="14">
-        <v>30016.7361197</v>
+        <v>30016.7168749</v>
       </c>
       <c r="H13" s="14">
-        <v>35382.2623902</v>
+        <v>35382.2376697</v>
       </c>
       <c r="I13" s="14">
-        <v>42553.5563617</v>
+        <v>42553.530931</v>
       </c>
       <c r="J13" s="14">
-        <v>51634.759898</v>
+        <v>51634.744893</v>
       </c>
       <c r="K13" s="14">
-        <v>46328.676746</v>
+        <v>46328.67124</v>
       </c>
       <c r="L13" s="14">
-        <v>54321.493129</v>
+        <v>54321.490578</v>
       </c>
       <c r="M13" s="14">
-        <v>73817.319409</v>
+        <v>73817.316935</v>
       </c>
       <c r="N13" s="14">
-        <v>78956.975377</v>
+        <v>78956.972014</v>
       </c>
       <c r="O13" s="14">
-        <v>78420.428584</v>
+        <v>78420.426577</v>
       </c>
       <c r="P13" s="14">
-        <v>75609.984831</v>
+        <v>75609.983217</v>
       </c>
       <c r="Q13" s="14">
-        <v>58166.478945</v>
+        <v>58166.47657</v>
       </c>
       <c r="R13" s="14">
-        <v>54747.612864</v>
+        <v>54747.60771</v>
       </c>
       <c r="S13" s="14">
-        <v>62655.0733</v>
+        <v>62655.066192</v>
       </c>
       <c r="T13" s="14">
-        <v>68799.744203</v>
+        <v>68799.732056</v>
       </c>
       <c r="U13" s="14">
-        <v>68317.369924</v>
+        <v>68318.338788</v>
       </c>
       <c r="V13" s="14">
-        <v>52420.203693</v>
+        <v>52420.199987</v>
       </c>
       <c r="W13" s="14">
-        <v>68776.173663</v>
+        <v>68782.564587</v>
       </c>
       <c r="X13" s="14">
-        <v>93756.617562</v>
-      </c>
-      <c r="Y13" s="15">
-        <v>67733.792983</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="15.06" customHeight="1">
+        <v>93942.767186</v>
+      </c>
+      <c r="Y13" s="14">
+        <v>91475.625337</v>
+      </c>
+      <c r="Z13" s="15">
+        <v>22052.259257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.06" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="11">
         <v>17902.3472768</v>
@@ -1491,18 +1505,21 @@
         <v>61687.013473</v>
       </c>
       <c r="W14" s="11">
-        <v>86727.359332</v>
+        <v>86731.967552</v>
       </c>
       <c r="X14" s="11">
-        <v>115089.880499</v>
-      </c>
-      <c r="Y14" s="12">
-        <v>74825.720036</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15.06" customHeight="1">
+        <v>115147.753503</v>
+      </c>
+      <c r="Y14" s="11">
+        <v>100629.399828</v>
+      </c>
+      <c r="Z14" s="12">
+        <v>23976.293748</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.06" customHeight="1">
       <c r="A15" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="14">
         <v>1328.66691385</v>
@@ -1568,18 +1585,21 @@
         <v>-13104.751155</v>
       </c>
       <c r="W15" s="14">
-        <v>-20002.465234</v>
+        <v>-20000.67916</v>
       </c>
       <c r="X15" s="14">
-        <v>-16584.996736</v>
-      </c>
-      <c r="Y15" s="15">
-        <v>-6015.319033</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="15.06" customHeight="1">
+        <v>-16426.931537</v>
+      </c>
+      <c r="Y15" s="14">
+        <v>-7989.361891</v>
+      </c>
+      <c r="Z15" s="15">
+        <v>-1932.05188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.06" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="11">
         <v>15806.6650611</v>
@@ -1645,18 +1665,21 @@
         <v>38223.6324565</v>
       </c>
       <c r="W16" s="11">
-        <v>50907.04606</v>
+        <v>50913.440354</v>
       </c>
       <c r="X16" s="11">
-        <v>73101.243988</v>
-      </c>
-      <c r="Y16" s="12">
-        <v>50629.411365</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" ht="15.06" customHeight="1">
+        <v>73286.691546</v>
+      </c>
+      <c r="Y16" s="11">
+        <v>68285.809149</v>
+      </c>
+      <c r="Z16" s="12">
+        <v>16032.280695</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="15.06" customHeight="1">
       <c r="A17" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="14">
         <v>14477.9981474</v>
@@ -1722,18 +1745,21 @@
         <v>51328.383612</v>
       </c>
       <c r="W17" s="14">
-        <v>70909.511294</v>
+        <v>70914.119513</v>
       </c>
       <c r="X17" s="14">
-        <v>89686.240724</v>
-      </c>
-      <c r="Y17" s="15">
-        <v>56644.730397</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" ht="15.06" customHeight="1">
+        <v>89713.623084</v>
+      </c>
+      <c r="Y17" s="14">
+        <v>76275.171039</v>
+      </c>
+      <c r="Z17" s="15">
+        <v>17964.332575</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="15.06" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" s="11">
         <v>2702.19562894</v>
@@ -1802,15 +1828,18 @@
         <v>-13983.64129</v>
       </c>
       <c r="X18" s="11">
-        <v>-12177.548953</v>
-      </c>
-      <c r="Y18" s="12">
-        <v>-4928.351008</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="15.06" customHeight="1">
+        <v>-12178.24898</v>
+      </c>
+      <c r="Y18" s="11">
+        <v>-6731.578921</v>
+      </c>
+      <c r="Z18" s="12">
+        <v>-2056.620062</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="15.06" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" s="14">
         <v>13744.6947415</v>
@@ -1879,15 +1908,18 @@
         <v>42735.5744459</v>
       </c>
       <c r="X19" s="14">
-        <v>59474.151692</v>
-      </c>
-      <c r="Y19" s="15">
-        <v>39470.778813</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" ht="15.06" customHeight="1">
+        <v>59473.45166</v>
+      </c>
+      <c r="Y19" s="14">
+        <v>52641.920271</v>
+      </c>
+      <c r="Z19" s="15">
+        <v>11781.469115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.06" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" s="11">
         <v>11042.4991125</v>
@@ -1956,15 +1988,18 @@
         <v>56719.215737</v>
       </c>
       <c r="X20" s="11">
-        <v>71651.700644</v>
-      </c>
-      <c r="Y20" s="12">
-        <v>44399.129821</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" ht="15.06" customHeight="1">
+        <v>71651.70064</v>
+      </c>
+      <c r="Y20" s="11">
+        <v>59373.499192</v>
+      </c>
+      <c r="Z20" s="12">
+        <v>13838.089177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="15.06" customHeight="1">
       <c r="A21" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="14">
         <v>-1373.528715</v>
@@ -2030,18 +2065,21 @@
         <v>-4234.9630923</v>
       </c>
       <c r="W21" s="14">
-        <v>-6018.823945</v>
+        <v>-6017.037869</v>
       </c>
       <c r="X21" s="14">
-        <v>-4407.4477836</v>
-      </c>
-      <c r="Y21" s="15">
-        <v>-1086.9680249</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="15.06" customHeight="1">
+        <v>-4248.6825563</v>
+      </c>
+      <c r="Y21" s="14">
+        <v>-1257.7829699</v>
+      </c>
+      <c r="Z21" s="15">
+        <v>124.56818233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15.06" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="11">
         <v>2061.97031969</v>
@@ -2107,18 +2145,21 @@
         <v>5914.66526126</v>
       </c>
       <c r="W22" s="11">
-        <v>8171.4716133</v>
+        <v>8177.865908</v>
       </c>
       <c r="X22" s="11">
-        <v>13627.0922958</v>
-      </c>
-      <c r="Y22" s="12">
-        <v>11158.6325511</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="15.06" customHeight="1">
+        <v>13813.2398855</v>
+      </c>
+      <c r="Y22" s="11">
+        <v>15643.8888785</v>
+      </c>
+      <c r="Z22" s="12">
+        <v>4250.8115806</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="15.06" customHeight="1">
       <c r="A23" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23" s="14">
         <v>3435.49903477</v>
@@ -2184,172 +2225,181 @@
         <v>10149.6283536</v>
       </c>
       <c r="W23" s="14">
-        <v>14190.2955581</v>
+        <v>14194.9037773</v>
       </c>
       <c r="X23" s="14">
-        <v>18034.5400791</v>
-      </c>
-      <c r="Y23" s="15">
-        <v>12245.600576</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="15.06" customHeight="1">
+        <v>18061.9224427</v>
+      </c>
+      <c r="Y23" s="14">
+        <v>16901.6718484</v>
+      </c>
+      <c r="Z23" s="15">
+        <v>4126.2433982</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="15.06" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="11">
         <v>-2156.4418231</v>
       </c>
       <c r="C24" s="11">
-        <v>-2423.7799709</v>
+        <v>-2423.7931397</v>
       </c>
       <c r="D24" s="11">
-        <v>-2631.3702684</v>
+        <v>-2631.3791619</v>
       </c>
       <c r="E24" s="11">
-        <v>-3187.7707366</v>
+        <v>-3187.7774985</v>
       </c>
       <c r="F24" s="11">
-        <v>-4015.6722234</v>
+        <v>-4015.6816314</v>
       </c>
       <c r="G24" s="11">
-        <v>-5339.023943</v>
+        <v>-5339.043189</v>
       </c>
       <c r="H24" s="11">
-        <v>-5753.659192</v>
+        <v>-5753.683912</v>
       </c>
       <c r="I24" s="11">
-        <v>-7861.032359</v>
+        <v>-7861.057789</v>
       </c>
       <c r="J24" s="11">
-        <v>-9649.494484</v>
+        <v>-9649.509489</v>
       </c>
       <c r="K24" s="11">
-        <v>-8185.516727</v>
+        <v>-8185.522232</v>
       </c>
       <c r="L24" s="11">
-        <v>-10996.289968</v>
+        <v>-10996.292518</v>
       </c>
       <c r="M24" s="11">
-        <v>-15313.133062</v>
+        <v>-15313.135535</v>
       </c>
       <c r="N24" s="11">
-        <v>-15007.669375</v>
+        <v>-15007.67274</v>
       </c>
       <c r="O24" s="11">
-        <v>-14001.519654</v>
+        <v>-14001.521661</v>
       </c>
       <c r="P24" s="11">
-        <v>-12107.911235</v>
+        <v>-12107.912849</v>
       </c>
       <c r="Q24" s="11">
-        <v>-5449.5555333</v>
+        <v>-5449.5579077</v>
       </c>
       <c r="R24" s="11">
-        <v>-5312.189835</v>
+        <v>-5312.19499</v>
       </c>
       <c r="S24" s="11">
-        <v>-8046.202127</v>
+        <v>-8046.209235</v>
       </c>
       <c r="T24" s="11">
-        <v>-11442.167424</v>
+        <v>-11442.179571</v>
       </c>
       <c r="U24" s="11">
-        <v>-9716.875189</v>
+        <v>-9715.906324</v>
       </c>
       <c r="V24" s="11">
-        <v>-4949.881388</v>
+        <v>-4949.885095</v>
       </c>
       <c r="W24" s="11">
-        <v>-8723.255528</v>
+        <v>-8723.258899</v>
       </c>
       <c r="X24" s="11">
-        <v>-17056.513574</v>
-      </c>
-      <c r="Y24" s="12">
-        <v>-10564.647166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="15.06" customHeight="1">
+        <v>-17086.302154</v>
+      </c>
+      <c r="Y24" s="11">
+        <v>-14100.023255</v>
+      </c>
+      <c r="Z24" s="12">
+        <v>-3324.107029</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="15.06" customHeight="1">
       <c r="A25" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="14">
         <v>1029.69825146</v>
       </c>
       <c r="C25" s="14">
-        <v>899.9605089</v>
+        <v>899.94734015</v>
       </c>
       <c r="D25" s="14">
-        <v>702.98834312</v>
+        <v>702.97944962</v>
       </c>
       <c r="E25" s="14">
-        <v>562.01572447</v>
+        <v>562.00896247</v>
       </c>
       <c r="F25" s="14">
-        <v>709.55448466</v>
+        <v>709.54507666</v>
       </c>
       <c r="G25" s="14">
-        <v>1009.68835832</v>
+        <v>1009.66911357</v>
       </c>
       <c r="H25" s="14">
-        <v>1512.47354483</v>
+        <v>1512.44882433</v>
       </c>
       <c r="I25" s="14">
-        <v>1847.10557331</v>
+        <v>1847.08014231</v>
       </c>
       <c r="J25" s="14">
-        <v>1852.96801425</v>
+        <v>1852.95300896</v>
       </c>
       <c r="K25" s="14">
-        <v>1781.37867588</v>
+        <v>1781.37316983</v>
       </c>
       <c r="L25" s="14">
-        <v>1913.34319996</v>
+        <v>1913.34064963</v>
       </c>
       <c r="M25" s="14">
-        <v>2954.45777683</v>
+        <v>2954.45530247</v>
       </c>
       <c r="N25" s="14">
-        <v>3851.36672035</v>
+        <v>3851.36335662</v>
       </c>
       <c r="O25" s="14">
-        <v>3846.37330644</v>
+        <v>3846.37129921</v>
       </c>
       <c r="P25" s="14">
-        <v>4412.03726477</v>
+        <v>4412.03565073</v>
       </c>
       <c r="Q25" s="14">
-        <v>4594.795863</v>
+        <v>4594.7934885</v>
       </c>
       <c r="R25" s="14">
-        <v>4993.9911393</v>
+        <v>4993.9859841</v>
       </c>
       <c r="S25" s="14">
-        <v>5576.6211346</v>
+        <v>5576.6140263</v>
       </c>
       <c r="T25" s="14">
-        <v>6177.2168502</v>
+        <v>6177.204704</v>
       </c>
       <c r="U25" s="14">
-        <v>6976.14744</v>
+        <v>6977.1163039</v>
       </c>
       <c r="V25" s="14">
-        <v>4542.6176761</v>
+        <v>4542.6139684</v>
       </c>
       <c r="W25" s="14">
-        <v>5932.2756731</v>
+        <v>5932.2723028</v>
       </c>
       <c r="X25" s="14">
-        <v>6974.1950243</v>
-      </c>
-      <c r="Y25" s="15">
-        <v>6547.2269398</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" ht="15.06" customHeight="1">
+        <v>6974.8970892</v>
+      </c>
+      <c r="Y25" s="14">
+        <v>8777.2042005</v>
+      </c>
+      <c r="Z25" s="15">
+        <v>2283.1593159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="15.06" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="11">
         <v>3186.14007468</v>
@@ -2418,15 +2468,18 @@
         <v>14655.5312023</v>
       </c>
       <c r="X26" s="11">
-        <v>24030.708598</v>
-      </c>
-      <c r="Y26" s="12">
-        <v>17111.8741064</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" ht="15.06" customHeight="1">
+        <v>24061.199243</v>
+      </c>
+      <c r="Y26" s="11">
+        <v>22877.2274555</v>
+      </c>
+      <c r="Z26" s="12">
+        <v>5607.2663449</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="15.06" customHeight="1">
       <c r="A27" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="14">
         <v>1673.17899242</v>
@@ -2497,13 +2550,16 @@
       <c r="X27" s="14">
         <v>12308.2473735</v>
       </c>
-      <c r="Y27" s="15">
-        <v>9488.0391467</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y27" s="14">
+        <v>12935.6106551</v>
+      </c>
+      <c r="Z27" s="15">
+        <v>3332.1244177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="15.06" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="11">
         <v>1911.38804725</v>
@@ -2574,13 +2630,16 @@
       <c r="X28" s="11">
         <v>13681.1785508</v>
       </c>
-      <c r="Y28" s="12">
-        <v>10557.1546796</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y28" s="11">
+        <v>14412.6119872</v>
+      </c>
+      <c r="Z28" s="12">
+        <v>3736.8192457</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="15.06" customHeight="1">
       <c r="A29" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="14">
         <v>238.209054829</v>
@@ -2651,19 +2710,22 @@
       <c r="X29" s="14">
         <v>1372.93117733</v>
       </c>
-      <c r="Y29" s="15">
-        <v>1069.11553273</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y29" s="14">
+        <v>1477.00133201</v>
+      </c>
+      <c r="Z29" s="15">
+        <v>404.694828</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="15.06" customHeight="1">
       <c r="A30" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" s="11">
         <v>849.656832889</v>
       </c>
       <c r="C30" s="11">
-        <v>-1228.2241176</v>
+        <v>-1228.7141176</v>
       </c>
       <c r="D30" s="11">
         <v>-1165.68097888</v>
@@ -2726,15 +2788,18 @@
         <v>-16693.127239</v>
       </c>
       <c r="X30" s="11">
-        <v>-20466.224344</v>
-      </c>
-      <c r="Y30" s="12">
-        <v>-6799.986208</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="15.06" customHeight="1">
+        <v>-20465.947511</v>
+      </c>
+      <c r="Y30" s="11">
+        <v>-8285.355966</v>
+      </c>
+      <c r="Z30" s="12">
+        <v>-1397.278612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="15.06" customHeight="1">
       <c r="A31" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" s="14">
         <v>-2111.1133955</v>
@@ -2803,15 +2868,18 @@
         <v>-6380.521503</v>
       </c>
       <c r="X31" s="14">
-        <v>-13799.28254</v>
-      </c>
-      <c r="Y31" s="15">
-        <v>-12224.878507</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="15.06" customHeight="1">
+        <v>-13799.005708</v>
+      </c>
+      <c r="Y31" s="14">
+        <v>-15971.96182</v>
+      </c>
+      <c r="Z31" s="15">
+        <v>-2533.386536</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="15.06" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" s="11">
         <v>325.34652795</v>
@@ -2880,15 +2948,18 @@
         <v>3180.81377367</v>
       </c>
       <c r="X32" s="11">
-        <v>3383.23880992</v>
-      </c>
-      <c r="Y32" s="12">
-        <v>571.67031019</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" ht="15.06" customHeight="1">
+        <v>3383.51564264</v>
+      </c>
+      <c r="Y32" s="11">
+        <v>1174.89190221</v>
+      </c>
+      <c r="Z32" s="12">
+        <v>1087.0712322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="15.06" customHeight="1">
       <c r="A33" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B33" s="14">
         <v>325.34652795</v>
@@ -2957,15 +3028,18 @@
         <v>2924.0146046</v>
       </c>
       <c r="X33" s="14">
-        <v>2840.16744347</v>
-      </c>
-      <c r="Y33" s="15">
-        <v>860.98974037</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" ht="15.06" customHeight="1">
+        <v>2840.44427625</v>
+      </c>
+      <c r="Y33" s="14">
+        <v>1610.06114332</v>
+      </c>
+      <c r="Z33" s="15">
+        <v>903.55159055</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="15.06" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="11">
         <v>0.0</v>
@@ -3036,13 +3110,16 @@
       <c r="X34" s="11">
         <v>543.07136643</v>
       </c>
-      <c r="Y34" s="12">
-        <v>-289.3194302</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y34" s="11">
+        <v>-435.16924112</v>
+      </c>
+      <c r="Z34" s="12">
+        <v>183.5196417</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="15.06" customHeight="1">
       <c r="A35" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="14">
         <v>2436.45992343</v>
@@ -3113,13 +3190,16 @@
       <c r="X35" s="14">
         <v>17182.5213499</v>
       </c>
-      <c r="Y35" s="15">
-        <v>12796.5488172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y35" s="14">
+        <v>17146.8537218</v>
+      </c>
+      <c r="Z35" s="15">
+        <v>3620.4577687</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="15.06" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B36" s="11">
         <v>2394.76910306</v>
@@ -3190,13 +3270,16 @@
       <c r="X36" s="11">
         <v>14227.4357768</v>
       </c>
-      <c r="Y36" s="12">
-        <v>10655.7576692</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y36" s="11">
+        <v>14224.2551407</v>
+      </c>
+      <c r="Z36" s="12">
+        <v>3245.1641644</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="15.06" customHeight="1">
       <c r="A37" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" s="14">
         <v>41.69082037</v>
@@ -3267,13 +3350,16 @@
       <c r="X37" s="14">
         <v>2955.08557313</v>
       </c>
-      <c r="Y37" s="15">
-        <v>2140.79114795</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y37" s="14">
+        <v>2922.59858113</v>
+      </c>
+      <c r="Z37" s="15">
+        <v>375.29360429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" ht="15.06" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B38" s="11">
         <v>-174.69070286</v>
@@ -3344,13 +3430,16 @@
       <c r="X38" s="11">
         <v>427.0013722</v>
       </c>
-      <c r="Y38" s="12">
-        <v>7151.6687862</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y38" s="11">
+        <v>8722.6924292</v>
+      </c>
+      <c r="Z38" s="12">
+        <v>1588.5224358</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" ht="15.06" customHeight="1">
       <c r="A39" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39" s="14">
         <v>1278.68457942</v>
@@ -3421,13 +3510,16 @@
       <c r="X39" s="14">
         <v>3306.82731523</v>
       </c>
-      <c r="Y39" s="15">
-        <v>6170.4028732</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y39" s="14">
+        <v>9839.5426682</v>
+      </c>
+      <c r="Z39" s="15">
+        <v>2171.8158946</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" ht="15.06" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B40" s="11">
         <v>0.0</v>
@@ -3498,13 +3590,16 @@
       <c r="X40" s="11">
         <v>1056.12523936</v>
       </c>
-      <c r="Y40" s="12">
-        <v>3541.91446633</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y40" s="11">
+        <v>5168.94291318</v>
+      </c>
+      <c r="Z40" s="12">
+        <v>1447.0602161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="15.06" customHeight="1">
       <c r="A41" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B41" s="14">
         <v>1278.68457942</v>
@@ -3575,13 +3670,16 @@
       <c r="X41" s="14">
         <v>2250.70207581</v>
       </c>
-      <c r="Y41" s="15">
-        <v>2628.4884068</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y41" s="14">
+        <v>4670.5997549</v>
+      </c>
+      <c r="Z41" s="15">
+        <v>724.75567847</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" ht="15.06" customHeight="1">
       <c r="A42" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42" s="11">
         <v>1453.37528238</v>
@@ -3652,13 +3750,16 @@
       <c r="X42" s="11">
         <v>2879.825943058</v>
       </c>
-      <c r="Y42" s="12">
-        <v>-981.26591313</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y42" s="11">
+        <v>1116.85023877</v>
+      </c>
+      <c r="Z42" s="12">
+        <v>583.2934588</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" ht="15.06" customHeight="1">
       <c r="A43" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B43" s="14">
         <v>16.90193019</v>
@@ -3729,13 +3830,16 @@
       <c r="X43" s="14">
         <v>-551.034485885</v>
       </c>
-      <c r="Y43" s="15">
-        <v>80.331685522</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y43" s="14">
+        <v>19.923914044</v>
+      </c>
+      <c r="Z43" s="15">
+        <v>4.4128011487</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" ht="15.06" customHeight="1">
       <c r="A44" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B44" s="11">
         <v>1436.47335219</v>
@@ -3806,13 +3910,16 @@
       <c r="X44" s="11">
         <v>3430.86042893</v>
       </c>
-      <c r="Y44" s="12">
-        <v>-1061.59759874</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y44" s="11">
+        <v>1096.92632466</v>
+      </c>
+      <c r="Z44" s="12">
+        <v>578.88065765</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" ht="15.06" customHeight="1">
       <c r="A45" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B45" s="14">
         <v>121.958325998</v>
@@ -3883,13 +3990,16 @@
       <c r="X45" s="14">
         <v>823.340570674</v>
       </c>
-      <c r="Y45" s="15">
-        <v>-1694.023842</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y45" s="14">
+        <v>-2574.5881249</v>
+      </c>
+      <c r="Z45" s="15">
+        <v>-575.1720499</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" ht="15.06" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46" s="11">
         <v>0.0</v>
@@ -3960,13 +4070,16 @@
       <c r="X46" s="11">
         <v>-481.1669326</v>
       </c>
-      <c r="Y46" s="12">
-        <v>-1694.023842</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y46" s="11">
+        <v>-2574.5881249</v>
+      </c>
+      <c r="Z46" s="12">
+        <v>-575.1720499</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" ht="15.06" customHeight="1">
       <c r="A47" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="14">
         <v>-121.958326</v>
@@ -4037,19 +4150,22 @@
       <c r="X47" s="14">
         <v>-1304.5075033</v>
       </c>
-      <c r="Y47" s="15">
+      <c r="Y47" s="14">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Z47" s="15">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" ht="15.06" customHeight="1">
       <c r="A48" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B48" s="11">
         <v>2151.47868287</v>
       </c>
       <c r="C48" s="11">
-        <v>1066.49468491</v>
+        <v>1066.00468491</v>
       </c>
       <c r="D48" s="11">
         <v>-464.511147526</v>
@@ -4114,19 +4230,22 @@
       <c r="X48" s="11">
         <v>-8488.174641</v>
       </c>
-      <c r="Y48" s="12">
-        <v>-1255.0340707</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y48" s="11">
+        <v>-179.88640261</v>
+      </c>
+      <c r="Z48" s="12">
+        <v>-828.6170869</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="15.06" customHeight="1">
       <c r="A49" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" s="14">
         <v>444.64015126</v>
       </c>
       <c r="C49" s="14">
-        <v>905.962389026</v>
+        <v>905.472389026</v>
       </c>
       <c r="D49" s="14">
         <v>-1704.62415402</v>
@@ -4191,13 +4310,16 @@
       <c r="X49" s="14">
         <v>4084.40709501</v>
       </c>
-      <c r="Y49" s="15">
-        <v>1332.500729508</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y49" s="14">
+        <v>4003.170087036</v>
+      </c>
+      <c r="Z49" s="15">
+        <v>-1321.42519</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" ht="15.06" customHeight="1">
       <c r="A50" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50" s="11">
         <v>-1706.83853118</v>
@@ -4268,13 +4390,16 @@
       <c r="X50" s="11">
         <v>12572.581736</v>
       </c>
-      <c r="Y50" s="12">
-        <v>2587.5348001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y50" s="11">
+        <v>4183.05648921</v>
+      </c>
+      <c r="Z50" s="12">
+        <v>-492.8081033</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" ht="15.06" customHeight="1">
       <c r="A51" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B51" s="14">
         <v>862.02392241</v>
@@ -4345,96 +4470,102 @@
       <c r="X51" s="14">
         <v>570.89089449</v>
       </c>
-      <c r="Y51" s="15">
-        <v>1222.28142538</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" ht="15.06" customHeight="1">
+      <c r="Y51" s="14">
+        <v>1718.38795211</v>
+      </c>
+      <c r="Z51" s="15">
+        <v>951.37462549</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" ht="15.06" customHeight="1">
       <c r="A52" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B52" s="11">
         <v>4.252749824</v>
       </c>
       <c r="C52" s="11">
-        <v>-187.909365663</v>
+        <v>-188.386196863</v>
       </c>
       <c r="D52" s="11">
-        <v>123.512797416</v>
+        <v>123.521690916</v>
       </c>
       <c r="E52" s="11">
-        <v>71.42355943</v>
+        <v>71.43032143</v>
       </c>
       <c r="F52" s="11">
-        <v>59.41589915</v>
+        <v>59.42530715</v>
       </c>
       <c r="G52" s="11">
-        <v>440.487996557</v>
+        <v>440.507241307</v>
       </c>
       <c r="H52" s="11">
-        <v>127.397087622</v>
+        <v>127.421808072</v>
       </c>
       <c r="I52" s="11">
-        <v>495.03320105</v>
+        <v>495.05863205</v>
       </c>
       <c r="J52" s="11">
-        <v>-424.48594605</v>
+        <v>-424.47094075</v>
       </c>
       <c r="K52" s="11">
-        <v>-545.0039415</v>
+        <v>-544.99843541</v>
       </c>
       <c r="L52" s="11">
-        <v>-748.79540256</v>
+        <v>-748.79285238</v>
       </c>
       <c r="M52" s="11">
-        <v>1027.18065435</v>
+        <v>1027.18312873</v>
       </c>
       <c r="N52" s="11">
-        <v>87.110901028</v>
+        <v>87.114264733</v>
       </c>
       <c r="O52" s="11">
-        <v>625.51443975</v>
+        <v>625.51644698</v>
       </c>
       <c r="P52" s="11">
-        <v>526.488198282</v>
+        <v>526.489812479</v>
       </c>
       <c r="Q52" s="11">
-        <v>642.498984325</v>
+        <v>642.501358827</v>
       </c>
       <c r="R52" s="11">
-        <v>247.182701957</v>
+        <v>247.187857333</v>
       </c>
       <c r="S52" s="11">
-        <v>299.44236995</v>
+        <v>299.44947828</v>
       </c>
       <c r="T52" s="11">
-        <v>1087.09495614</v>
+        <v>1087.10710232</v>
       </c>
       <c r="U52" s="11">
-        <v>1511.31006795</v>
+        <v>1510.34120411</v>
       </c>
       <c r="V52" s="11">
-        <v>1153.345738266</v>
+        <v>1153.349445918</v>
       </c>
       <c r="W52" s="11">
-        <v>1258.05843061</v>
+        <v>1256.27572558</v>
       </c>
       <c r="X52" s="11">
-        <v>867.03859251</v>
-      </c>
-      <c r="Y52" s="12">
-        <v>291.94084441</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" ht="15.06" customHeight="1">
+        <v>739.03880664</v>
+      </c>
+      <c r="Y52" s="11">
+        <v>868.41852556</v>
+      </c>
+      <c r="Z52" s="12">
+        <v>526.75587917</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" ht="15.06" customHeight="1">
       <c r="A53" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B53" s="14">
         <v>-12.367089521</v>
       </c>
       <c r="C53" s="14">
-        <v>-2454.11240919</v>
+        <v>-2454.60240919</v>
       </c>
       <c r="D53" s="14">
         <v>-1304.41319305</v>
@@ -4497,10 +4628,13 @@
         <v>-17346.6724111</v>
       </c>
       <c r="X53" s="14">
-        <v>-21037.11523849</v>
-      </c>
-      <c r="Y53" s="15">
-        <v>-8022.26763338</v>
+        <v>-21036.83840549</v>
+      </c>
+      <c r="Y53" s="14">
+        <v>-10003.74391811</v>
+      </c>
+      <c r="Z53" s="15">
+        <v>-2348.65323749</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -4510,7 +4644,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
@@ -4526,7 +4660,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -4542,7 +4676,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -4558,7 +4692,7 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -4574,7 +4708,7 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -4606,7 +4740,7 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -4622,7 +4756,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -4638,7 +4772,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -4654,7 +4788,7 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -4686,7 +4820,7 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -4718,7 +4852,7 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -4734,7 +4868,7 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -4766,7 +4900,7 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -4816,7 +4950,7 @@
   <mergeCells count="22">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B10:Y10"/>
+    <mergeCell ref="B10:Z10"/>
     <mergeCell ref="A55:L55"/>
     <mergeCell ref="A56:L56"/>
     <mergeCell ref="A57:L57"/>

</xml_diff>